<commit_message>
Now creates tournament codes for RoundRobin tournament
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lette\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A07F98-67D2-4565-BE59-8C03856B55A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790255B3-A1BD-4C73-A478-25E428FE1010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3610" yWindow="2350" windowWidth="28800" windowHeight="15460" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
+    <workbookView xWindow="1467" yWindow="1467" windowWidth="19200" windowHeight="10073" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="119">
   <si>
     <t>Team Fire</t>
   </si>
@@ -379,6 +379,18 @@
   </si>
   <si>
     <t>Foxx Bear</t>
+  </si>
+  <si>
+    <t>GOKU177</t>
+  </si>
+  <si>
+    <t>H0K1M0K1</t>
+  </si>
+  <si>
+    <t>H4RDR0CK</t>
+  </si>
+  <si>
+    <t>GUYFRD</t>
   </si>
 </sst>
 </file>
@@ -423,7 +435,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -517,11 +529,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -548,6 +573,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,37 +891,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B2ED7ED-18A8-44B1-83A1-7B4BE38C35CE}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="8" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.54296875" customWidth="1"/>
-    <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.703125" customWidth="1"/>
+    <col min="2" max="2" width="11.8203125" customWidth="1"/>
+    <col min="3" max="3" width="15.46875" customWidth="1"/>
+    <col min="4" max="4" width="19.05859375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.46875" customWidth="1"/>
+    <col min="6" max="6" width="18.29296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.3515625" customWidth="1"/>
+    <col min="8" max="8" width="19.64453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.52734375" customWidth="1"/>
+    <col min="10" max="10" width="18.17578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.8203125" customWidth="1"/>
+    <col min="12" max="12" width="14.46875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" customWidth="1"/>
+    <col min="14" max="14" width="22.17578125" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="15.54296875" customWidth="1"/>
+    <col min="16" max="16" width="15.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -934,15 +963,12 @@
       <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -984,11 +1010,8 @@
       <c r="O2" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -1034,16 +1057,13 @@
       <c r="O3" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="P3" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>51</v>
@@ -1084,11 +1104,8 @@
       <c r="O4" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1111,13 +1128,13 @@
         <v>69</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>78</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>88</v>
@@ -1129,20 +1146,17 @@
         <v>97</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1184,11 +1198,13 @@
       <c r="O6" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P6" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="D11" s="10" t="s">
         <v>27</v>
       </c>
@@ -1208,7 +1224,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1228,7 +1244,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
       <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
@@ -1248,7 +1264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="43" x14ac:dyDescent="0.5">
       <c r="D15" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1284,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
       <c r="D16" t="s">
         <v>29</v>
       </c>
@@ -1282,7 +1298,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:14" x14ac:dyDescent="0.5">
       <c r="H17" t="s">
         <v>33</v>
       </c>
@@ -1293,9 +1309,40 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:14" x14ac:dyDescent="0.5">
       <c r="H18" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="8:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="22" spans="8:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="N22" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="8:14" x14ac:dyDescent="0.5">
+      <c r="N23" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="8:14" x14ac:dyDescent="0.5">
+      <c r="N24" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="8:14" x14ac:dyDescent="0.5">
+      <c r="N25" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="8:14" x14ac:dyDescent="0.5">
+      <c r="N26" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="8:14" x14ac:dyDescent="0.5">
+      <c r="N27" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished 'Current Standings' image creation; finished 'Round' image generation; Beginning to update match standings when JSON is received from callback
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lette\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790255B3-A1BD-4C73-A478-25E428FE1010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047FE7F8-5638-46D6-B499-44406A9133DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1467" yWindow="1467" windowWidth="19200" windowHeight="10073" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
+    <workbookView xWindow="3350" yWindow="2060" windowWidth="30700" windowHeight="15940" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -894,30 +894,30 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.703125" customWidth="1"/>
-    <col min="2" max="2" width="11.8203125" customWidth="1"/>
-    <col min="3" max="3" width="15.46875" customWidth="1"/>
-    <col min="4" max="4" width="19.05859375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.46875" customWidth="1"/>
-    <col min="6" max="6" width="18.29296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.3515625" customWidth="1"/>
-    <col min="8" max="8" width="19.64453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.52734375" customWidth="1"/>
-    <col min="10" max="10" width="18.17578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.8203125" customWidth="1"/>
-    <col min="12" max="12" width="14.46875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.36328125" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.54296875" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="22.17578125" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="15.52734375" customWidth="1"/>
+    <col min="16" max="16" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -964,7 +964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1199,12 +1199,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D11" s="10" t="s">
         <v>27</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="43" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>28</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>29</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.5">
+    <row r="17" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H17" t="s">
         <v>33</v>
       </c>
@@ -1309,38 +1309,38 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.5">
+    <row r="18" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="8:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="22" spans="8:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="8:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="8:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N22" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.5">
+    <row r="23" spans="8:14" x14ac:dyDescent="0.35">
       <c r="N23" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.5">
+    <row r="24" spans="8:14" x14ac:dyDescent="0.35">
       <c r="N24" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.5">
+    <row r="25" spans="8:14" x14ac:dyDescent="0.35">
       <c r="N25" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.5">
+    <row r="26" spans="8:14" x14ac:dyDescent="0.35">
       <c r="N26" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.5">
+    <row r="27" spans="8:14" x14ac:dyDescent="0.35">
       <c r="N27" s="4" t="s">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
Tournaments now correctly advance and finish. Match Tournament Codes are sent to the creator via private message in the Discord API
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lette\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1144916-0C93-4ADB-8E0E-4BEA664C7658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E7E4D8-E193-40F6-BC6C-3CA3AB48D929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="2400" windowWidth="30700" windowHeight="15940" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="122">
   <si>
     <t>Team Fire</t>
   </si>
@@ -90,307 +90,316 @@
     <t>Lusantia</t>
   </si>
   <si>
+    <t>Dspac3</t>
+  </si>
+  <si>
+    <t>Sir Squishington</t>
+  </si>
+  <si>
+    <t>Moone</t>
+  </si>
+  <si>
+    <t>gigabitsofwit</t>
+  </si>
+  <si>
+    <t>Essentia1Oil</t>
+  </si>
+  <si>
+    <t>Syntratic</t>
+  </si>
+  <si>
+    <t>CraftyGuy</t>
+  </si>
+  <si>
+    <t>KaleBrew</t>
+  </si>
+  <si>
+    <t>Tournament Type</t>
+  </si>
+  <si>
+    <t>ROUND_ROBIN</t>
+  </si>
+  <si>
+    <t>SINGLE_ELIMINATION</t>
+  </si>
+  <si>
+    <t>Team Size</t>
+  </si>
+  <si>
+    <t>Between 1 - 5</t>
+  </si>
+  <si>
+    <t>Pick Type</t>
+  </si>
+  <si>
+    <t>ALL_RANDOM</t>
+  </si>
+  <si>
+    <t>TOURNAMENT_DRAFT</t>
+  </si>
+  <si>
+    <t>BLIND_PICK</t>
+  </si>
+  <si>
+    <t>Map Type</t>
+  </si>
+  <si>
+    <t>Accepted Values:</t>
+  </si>
+  <si>
+    <t>DRAFT_MODE</t>
+  </si>
+  <si>
+    <t>TWISTED_TREELINE</t>
+  </si>
+  <si>
+    <t>HOWLING_ABYSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUMMONERS_RIFT </t>
+  </si>
+  <si>
+    <t>SUMMONERS_RIFT</t>
+  </si>
+  <si>
+    <t>Spectator Type</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>LOBBYONLY</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Tournament</t>
+  </si>
+  <si>
+    <t>TitaniumTitan43</t>
+  </si>
+  <si>
+    <t>Bbygrls</t>
+  </si>
+  <si>
+    <t>Dyrus Bot</t>
+  </si>
+  <si>
+    <t>TimesAndSeasons</t>
+  </si>
+  <si>
+    <t>Carpe Dio</t>
+  </si>
+  <si>
+    <t>kinlly</t>
+  </si>
+  <si>
+    <t>Crimsonn Chin</t>
+  </si>
+  <si>
+    <t>Dallin</t>
+  </si>
+  <si>
+    <t>Drubii</t>
+  </si>
+  <si>
+    <t>Dyronius</t>
+  </si>
+  <si>
+    <t>Furyoth</t>
+  </si>
+  <si>
+    <t>MonteCristo4</t>
+  </si>
+  <si>
+    <t>PacMySac</t>
+  </si>
+  <si>
+    <t>ProfDrMrFluffy</t>
+  </si>
+  <si>
+    <t>Salopek</t>
+  </si>
+  <si>
+    <t>Whitemamba100</t>
+  </si>
+  <si>
+    <t>Rageromer</t>
+  </si>
+  <si>
+    <t>adamtay11</t>
+  </si>
+  <si>
+    <t>Backen</t>
+  </si>
+  <si>
+    <t>Baekun</t>
+  </si>
+  <si>
+    <t>bunnrie</t>
+  </si>
+  <si>
+    <t>burdman96</t>
+  </si>
+  <si>
+    <t>D4rk Fr3nzy</t>
+  </si>
+  <si>
+    <t>Darth Kakarot</t>
+  </si>
+  <si>
+    <t>Derpin</t>
+  </si>
+  <si>
+    <t>Diabolical Newts</t>
+  </si>
+  <si>
+    <t>Eggcarton</t>
+  </si>
+  <si>
+    <t>FathomVoid</t>
+  </si>
+  <si>
+    <t>Hoodie Thief</t>
+  </si>
+  <si>
+    <t>ilaka akali</t>
+  </si>
+  <si>
+    <t>jaysm11</t>
+  </si>
+  <si>
+    <t>Jokkioxx</t>
+  </si>
+  <si>
+    <t>LapizDragon</t>
+  </si>
+  <si>
+    <t>McAirth</t>
+  </si>
+  <si>
+    <t>Momonosuke</t>
+  </si>
+  <si>
+    <t>PizzaFTK</t>
+  </si>
+  <si>
+    <t>potatosquid10</t>
+  </si>
+  <si>
+    <t>Qawzz</t>
+  </si>
+  <si>
+    <t>Reans Aura</t>
+  </si>
+  <si>
+    <t>Remmytastic</t>
+  </si>
+  <si>
+    <t>Ryfthunter</t>
+  </si>
+  <si>
+    <t>Sasha Smalls</t>
+  </si>
+  <si>
+    <t>The Hunt Is On</t>
+  </si>
+  <si>
+    <t>thelostkoopa</t>
+  </si>
+  <si>
+    <t>Troudge</t>
+  </si>
+  <si>
+    <t>Zithz</t>
+  </si>
+  <si>
+    <t>Ikazichi</t>
+  </si>
+  <si>
+    <t>Jkay13</t>
+  </si>
+  <si>
+    <t>Laeconian</t>
+  </si>
+  <si>
+    <t>Lay Down And Cry</t>
+  </si>
+  <si>
+    <t>Puppy Shark</t>
+  </si>
+  <si>
+    <t>Shadiee</t>
+  </si>
+  <si>
+    <t>starwarsfish</t>
+  </si>
+  <si>
+    <t>1 800 CRY MOAR</t>
+  </si>
+  <si>
+    <t>1koi</t>
+  </si>
+  <si>
+    <t>3llismore</t>
+  </si>
+  <si>
+    <t>69 me Vladdy</t>
+  </si>
+  <si>
+    <t>Acist</t>
+  </si>
+  <si>
+    <t>ADC Odeion</t>
+  </si>
+  <si>
+    <t>Archidamus</t>
+  </si>
+  <si>
+    <t>Armadillo</t>
+  </si>
+  <si>
+    <t>Arzir</t>
+  </si>
+  <si>
+    <t>Foxx Bear</t>
+  </si>
+  <si>
+    <t>GOKU177</t>
+  </si>
+  <si>
+    <t>H0K1M0K1</t>
+  </si>
+  <si>
+    <t>H4RDR0CK</t>
+  </si>
+  <si>
+    <t>GUYFRD</t>
+  </si>
+  <si>
+    <t>Bmuffin08</t>
+  </si>
+  <si>
+    <t>TournamentName</t>
+  </si>
+  <si>
+    <t>This is used to identify the tournament. Please make it unique if you are hosting multiple tournaments in your server at one time.</t>
+  </si>
+  <si>
+    <t>Create Channels</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>The Discord Bot requires CHANNEL_PERMISSIONS to create Categories and Channels. If you would not like the Bot to perform these actions, place NO in the field and the Bot will guide you through what is required</t>
+  </si>
+  <si>
     <t>Taegondy</t>
-  </si>
-  <si>
-    <t>Dspac3</t>
-  </si>
-  <si>
-    <t>Sir Squishington</t>
-  </si>
-  <si>
-    <t>Moone</t>
-  </si>
-  <si>
-    <t>gigabitsofwit</t>
-  </si>
-  <si>
-    <t>Essentia1Oil</t>
-  </si>
-  <si>
-    <t>Syntratic</t>
-  </si>
-  <si>
-    <t>CraftyGuy</t>
-  </si>
-  <si>
-    <t>KaleBrew</t>
-  </si>
-  <si>
-    <t>Tournament Type</t>
-  </si>
-  <si>
-    <t>ROUND_ROBIN</t>
-  </si>
-  <si>
-    <t>SINGLE_ELIMINATION</t>
-  </si>
-  <si>
-    <t>Team Size</t>
-  </si>
-  <si>
-    <t>Between 1 - 5</t>
-  </si>
-  <si>
-    <t>Pick Type</t>
-  </si>
-  <si>
-    <t>ALL_RANDOM</t>
-  </si>
-  <si>
-    <t>TOURNAMENT_DRAFT</t>
-  </si>
-  <si>
-    <t>BLIND_PICK</t>
-  </si>
-  <si>
-    <t>Map Type</t>
-  </si>
-  <si>
-    <t>Accepted Values:</t>
-  </si>
-  <si>
-    <t>DRAFT_MODE</t>
-  </si>
-  <si>
-    <t>TWISTED_TREELINE</t>
-  </si>
-  <si>
-    <t>HOWLING_ABYSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUMMONERS_RIFT </t>
-  </si>
-  <si>
-    <t>SUMMONERS_RIFT</t>
-  </si>
-  <si>
-    <t>Spectator Type</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>LOBBYONLY</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>MetaData</t>
-  </si>
-  <si>
-    <t>Anything really. Could be a description, could be your birthday, anything.</t>
-  </si>
-  <si>
-    <t>Tournament</t>
-  </si>
-  <si>
-    <t>TitaniumTitan43</t>
-  </si>
-  <si>
-    <t>Bbygrls</t>
-  </si>
-  <si>
-    <t>Dyrus Bot</t>
-  </si>
-  <si>
-    <t>TimesAndSeasons</t>
-  </si>
-  <si>
-    <t>Carpe Dio</t>
-  </si>
-  <si>
-    <t>kinlly</t>
-  </si>
-  <si>
-    <t>Crimsonn Chin</t>
-  </si>
-  <si>
-    <t>Dallin</t>
-  </si>
-  <si>
-    <t>DevolaPopola</t>
-  </si>
-  <si>
-    <t>Drubii</t>
-  </si>
-  <si>
-    <t>Dyronius</t>
-  </si>
-  <si>
-    <t>Furyoth</t>
-  </si>
-  <si>
-    <t>MonteCristo4</t>
-  </si>
-  <si>
-    <t>PacMySac</t>
-  </si>
-  <si>
-    <t>ProfDrMrFluffy</t>
-  </si>
-  <si>
-    <t>Salopek</t>
-  </si>
-  <si>
-    <t>Whitemamba100</t>
-  </si>
-  <si>
-    <t>Rageromer</t>
-  </si>
-  <si>
-    <t>adamtay11</t>
-  </si>
-  <si>
-    <t>Backen</t>
-  </si>
-  <si>
-    <t>Baekun</t>
-  </si>
-  <si>
-    <t>bunnrie</t>
-  </si>
-  <si>
-    <t>burdman96</t>
-  </si>
-  <si>
-    <t>D4rk Fr3nzy</t>
-  </si>
-  <si>
-    <t>Darth Kakarot</t>
-  </si>
-  <si>
-    <t>Derpin</t>
-  </si>
-  <si>
-    <t>Diabolical Newts</t>
-  </si>
-  <si>
-    <t>Eggcarton</t>
-  </si>
-  <si>
-    <t>FathomVoid</t>
-  </si>
-  <si>
-    <t>Hoodie Thief</t>
-  </si>
-  <si>
-    <t>ilaka akali</t>
-  </si>
-  <si>
-    <t>jaysm11</t>
-  </si>
-  <si>
-    <t>Jokkioxx</t>
-  </si>
-  <si>
-    <t>LapizDragon</t>
-  </si>
-  <si>
-    <t>McAirth</t>
-  </si>
-  <si>
-    <t>Momonosuke</t>
-  </si>
-  <si>
-    <t>PizzaFTK</t>
-  </si>
-  <si>
-    <t>potatosquid10</t>
-  </si>
-  <si>
-    <t>Qawzz</t>
-  </si>
-  <si>
-    <t>Reans Aura</t>
-  </si>
-  <si>
-    <t>Remmytastic</t>
-  </si>
-  <si>
-    <t>Ryfthunter</t>
-  </si>
-  <si>
-    <t>Sasha Smalls</t>
-  </si>
-  <si>
-    <t>The Hunt Is On</t>
-  </si>
-  <si>
-    <t>thelostkoopa</t>
-  </si>
-  <si>
-    <t>Troudge</t>
-  </si>
-  <si>
-    <t>Zithz</t>
-  </si>
-  <si>
-    <t>Ikazichi</t>
-  </si>
-  <si>
-    <t>Jkay13</t>
-  </si>
-  <si>
-    <t>Laeconian</t>
-  </si>
-  <si>
-    <t>Lay Down And Cry</t>
-  </si>
-  <si>
-    <t>Puppy Shark</t>
-  </si>
-  <si>
-    <t>Shadiee</t>
-  </si>
-  <si>
-    <t>starwarsfish</t>
-  </si>
-  <si>
-    <t>1 800 CRY MOAR</t>
-  </si>
-  <si>
-    <t>1koi</t>
-  </si>
-  <si>
-    <t>3llismore</t>
-  </si>
-  <si>
-    <t>69 me Vladdy</t>
-  </si>
-  <si>
-    <t>Acist</t>
-  </si>
-  <si>
-    <t>ADC Odeion</t>
-  </si>
-  <si>
-    <t>Archidamus</t>
-  </si>
-  <si>
-    <t>Armadillo</t>
-  </si>
-  <si>
-    <t>Arzir</t>
-  </si>
-  <si>
-    <t>Foxx Bear</t>
-  </si>
-  <si>
-    <t>GOKU177</t>
-  </si>
-  <si>
-    <t>H0K1M0K1</t>
-  </si>
-  <si>
-    <t>H4RDR0CK</t>
-  </si>
-  <si>
-    <t>GUYFRD</t>
-  </si>
-  <si>
-    <t>Bmuffin08</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -577,6 +586,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,7 +904,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,7 +912,7 @@
     <col min="1" max="1" width="15.7265625" customWidth="1"/>
     <col min="2" max="2" width="11.81640625" customWidth="1"/>
     <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="19.453125" customWidth="1"/>
     <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.36328125" customWidth="1"/>
@@ -936,215 +946,230 @@
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D11" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="3">
         <v>5</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" t="s">
         <v>38</v>
       </c>
-      <c r="J16" t="s">
-        <v>39</v>
-      </c>
       <c r="L16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D22" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="N22" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D23" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="N23" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.35">
       <c r="N24" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D25" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="N25" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>118</v>
+      </c>
       <c r="N26" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>119</v>
+      </c>
       <c r="N27" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1185,177 +1210,177 @@
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="E32" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="H32" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K32" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="L32" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C33" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="H33" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J33" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K33" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="L33" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="3:13" ht="26" x14ac:dyDescent="0.35">
       <c r="C34" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="H34" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K34" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="K34" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="L34" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C35" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J35" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K35" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="L35" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C36" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="G36" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beginning to implement single-elimination start function
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lette\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dallincawley/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E7E4D8-E193-40F6-BC6C-3CA3AB48D929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBFC5B1-05FB-A145-8F9D-D615B455BE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{B4BBD30C-308D-43C1-96DA-0B16C09D5273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -904,30 +895,30 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="8" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.54296875" customWidth="1"/>
-    <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" customWidth="1"/>
+    <col min="14" max="14" width="22.1640625" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="15.54296875" customWidth="1"/>
+    <col min="16" max="16" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -941,7 +932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -955,7 +946,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -969,7 +960,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -983,7 +974,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -997,7 +988,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1011,7 +1002,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D11" s="10" t="s">
         <v>26</v>
       </c>
@@ -1031,9 +1022,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F12" s="3">
         <v>5</v>
@@ -1051,7 +1042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D14" s="9" t="s">
         <v>36</v>
       </c>
@@ -1071,7 +1062,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>27</v>
       </c>
@@ -1091,7 +1082,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>28</v>
       </c>
@@ -1105,7 +1096,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="H17" t="s">
         <v>32</v>
       </c>
@@ -1116,13 +1107,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="H18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D22" s="14" t="s">
         <v>117</v>
       </c>
@@ -1130,7 +1121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1" t="s">
         <v>118</v>
       </c>
@@ -1138,12 +1129,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="N24" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D25" s="9" t="s">
         <v>36</v>
       </c>
@@ -1151,7 +1142,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>118</v>
       </c>
@@ -1159,7 +1150,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>119</v>
       </c>
@@ -1167,13 +1158,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="3:14" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:14" ht="144" x14ac:dyDescent="0.2">
       <c r="D29" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C31" s="7" t="s">
         <v>4</v>
       </c>
@@ -1208,7 +1199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C32" s="5" t="s">
         <v>55</v>
       </c>
@@ -1243,7 +1234,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C33" s="4" t="s">
         <v>56</v>
       </c>
@@ -1278,7 +1269,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="3:13" ht="26" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:13" ht="29" x14ac:dyDescent="0.2">
       <c r="C34" s="4" t="s">
         <v>57</v>
       </c>
@@ -1313,7 +1304,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
         <v>25</v>
       </c>
@@ -1348,7 +1339,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C36" s="4" t="s">
         <v>58</v>
       </c>

</xml_diff>